<commit_message>
Edit user test case
</commit_message>
<xml_diff>
--- a/src/test/resources/testDataFiles/SignUpData.xlsx
+++ b/src/test/resources/testDataFiles/SignUpData.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="28306"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="28129"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Yusuf Data\Study stuff\WorkSpace\Shaft_Engine_Practice\src\test\resources\testDataFiles\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\moham\eclipse-workspace\Shaft_Engine_Practice\src\test\resources\testDataFiles\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1114B288-A0F2-47BD-9D67-7C98D637E1BB}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{86B01729-AE49-4585-AA73-C837D82A0797}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11040" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -420,19 +420,19 @@
   <dimension ref="A1:F5"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F1" sqref="F1"/>
+      <selection activeCell="B1" sqref="B1:F5"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="14.6640625" customWidth="1"/>
+    <col min="1" max="1" width="14.7109375" customWidth="1"/>
     <col min="2" max="2" width="26" customWidth="1"/>
-    <col min="3" max="3" width="20.6640625" customWidth="1"/>
-    <col min="4" max="4" width="22.109375" customWidth="1"/>
-    <col min="5" max="6" width="15.6640625" customWidth="1"/>
+    <col min="3" max="3" width="20.7109375" customWidth="1"/>
+    <col min="4" max="4" width="22.140625" customWidth="1"/>
+    <col min="5" max="6" width="15.7109375" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -452,7 +452,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="2" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>6</v>
       </c>
@@ -472,7 +472,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="3" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>12</v>
       </c>
@@ -492,7 +492,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="4" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
         <v>15</v>
       </c>
@@ -512,7 +512,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="5" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
         <v>18</v>
       </c>

</xml_diff>